<commit_message>
More attention event testing.
</commit_message>
<xml_diff>
--- a/China/meta/example_attention_events.xlsx
+++ b/China/meta/example_attention_events.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="80">
   <si>
     <t>Event</t>
   </si>
@@ -275,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -289,11 +289,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -301,6 +303,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,21 +324,21 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -348,7 +352,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -362,7 +366,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -376,7 +380,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -390,7 +394,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -404,7 +408,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
@@ -418,7 +422,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B8">
@@ -432,7 +436,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B9">
@@ -446,7 +450,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B10">
@@ -460,7 +464,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B11">
@@ -474,7 +478,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B12">
@@ -488,7 +492,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B13">
@@ -502,7 +506,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B14">
@@ -516,7 +520,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B15">
@@ -530,7 +534,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B16">
@@ -544,7 +548,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B17">
@@ -558,7 +562,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B18">
@@ -572,7 +576,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B19">
@@ -586,7 +590,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B20">
@@ -600,7 +604,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B21">
@@ -614,7 +618,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B22">
@@ -628,7 +632,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B23">
@@ -642,7 +646,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B24">
@@ -656,7 +660,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B25">
@@ -670,7 +674,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B26">
@@ -684,7 +688,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B27">
@@ -698,7 +702,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B28">
@@ -712,7 +716,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B29">
@@ -726,7 +730,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B30">
@@ -740,7 +744,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B31">
@@ -754,7 +758,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B32">
@@ -768,7 +772,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B33">
@@ -782,7 +786,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B34">
@@ -796,7 +800,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B35">
@@ -810,7 +814,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B36">
@@ -824,7 +828,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B37">
@@ -838,7 +842,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B38">
@@ -852,7 +856,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B39">
@@ -866,7 +870,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B40">
@@ -880,7 +884,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B41">
@@ -894,7 +898,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B42">
@@ -908,7 +912,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B43">
@@ -922,7 +926,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B44">
@@ -936,7 +940,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B45">
@@ -950,7 +954,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B46">
@@ -964,7 +968,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B47">
@@ -978,7 +982,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B48">
@@ -992,7 +996,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B49">
@@ -1006,7 +1010,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B50">
@@ -1020,7 +1024,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B51">
@@ -1034,7 +1038,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B52">
@@ -1048,7 +1052,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B53">
@@ -1062,7 +1066,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B54">
@@ -1076,7 +1080,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B55">
@@ -1090,7 +1094,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B56">
@@ -1104,7 +1108,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B57">
@@ -1118,7 +1122,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B58">
@@ -1132,7 +1136,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B59">
@@ -1146,7 +1150,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B60">
@@ -1160,7 +1164,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B61">
@@ -1174,7 +1178,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B62">
@@ -1188,7 +1192,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B63">
@@ -1202,7 +1206,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B64">
@@ -1216,7 +1220,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B65">
@@ -1230,7 +1234,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B66">
@@ -1244,7 +1248,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B67">
@@ -1258,7 +1262,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B68">
@@ -1272,7 +1276,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B69">
@@ -1286,7 +1290,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B70">
@@ -1300,7 +1304,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B71">
@@ -1314,7 +1318,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B72">
@@ -1328,7 +1332,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B73">
@@ -1342,7 +1346,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B74">
@@ -1356,7 +1360,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B75">
@@ -1370,7 +1374,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B76">
@@ -1384,7 +1388,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B77">
@@ -1398,7 +1402,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B78">
@@ -1412,7 +1416,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B79">
@@ -1426,7 +1430,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B80">
@@ -1440,7 +1444,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B81">
@@ -1454,7 +1458,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B82">
@@ -1468,7 +1472,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B83">
@@ -1482,7 +1486,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B84">
@@ -1496,7 +1500,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B85">
@@ -1510,7 +1514,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B86">
@@ -1524,7 +1528,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B87">
@@ -1538,7 +1542,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B88">
@@ -1552,7 +1556,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B89">
@@ -1566,7 +1570,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B90">
@@ -1580,7 +1584,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B91">
@@ -1594,7 +1598,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B92">
@@ -1608,7 +1612,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B93">
@@ -1622,7 +1626,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B94">
@@ -1636,7 +1640,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B95">
@@ -1650,7 +1654,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B96">
@@ -1664,7 +1668,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B97">
@@ -1678,7 +1682,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B98">
@@ -1692,7 +1696,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B99">
@@ -1706,7 +1710,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B100">
@@ -1720,7 +1724,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B101">
@@ -1734,7 +1738,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B102">
@@ -1748,7 +1752,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B103">
@@ -1762,7 +1766,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B104">
@@ -1776,7 +1780,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B105">
@@ -1790,7 +1794,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B106">
@@ -1804,7 +1808,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B107">
@@ -1818,7 +1822,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B108">
@@ -1832,7 +1836,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B109">
@@ -1846,7 +1850,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B110">
@@ -1860,7 +1864,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B111">
@@ -1874,7 +1878,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B112">
@@ -1888,7 +1892,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B113">
@@ -1902,7 +1906,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B114">
@@ -1916,7 +1920,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B115">
@@ -1930,7 +1934,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B116">
@@ -1944,7 +1948,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B117">
@@ -1958,7 +1962,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B118">
@@ -1972,7 +1976,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B119">
@@ -1986,7 +1990,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B120">
@@ -2000,7 +2004,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B121">
@@ -2014,7 +2018,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B122">
@@ -2028,7 +2032,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B123">
@@ -2042,7 +2046,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B124">
@@ -2056,7 +2060,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B125">
@@ -2070,7 +2074,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B126">
@@ -2084,7 +2088,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B127">
@@ -2098,7 +2102,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B128">
@@ -2112,7 +2116,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B129">
@@ -2126,7 +2130,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B130">
@@ -2140,7 +2144,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B131">
@@ -2154,7 +2158,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B132">
@@ -2168,7 +2172,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B133">
@@ -2182,7 +2186,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B134">
@@ -2196,7 +2200,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B135">
@@ -2210,7 +2214,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="5" t="s">
+      <c r="A136" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B136">
@@ -2224,7 +2228,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B137">
@@ -2238,7 +2242,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="5" t="s">
+      <c r="A138" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B138">
@@ -2252,7 +2256,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="5" t="s">
+      <c r="A139" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B139">
@@ -2266,7 +2270,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B140">
@@ -2280,7 +2284,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="5" t="s">
+      <c r="A141" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B141">
@@ -2294,7 +2298,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B142">
@@ -2308,7 +2312,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="5" t="s">
+      <c r="A143" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B143">
@@ -2322,7 +2326,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="5" t="s">
+      <c r="A144" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B144">
@@ -2336,7 +2340,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="5" t="s">
+      <c r="A145" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B145">
@@ -2350,7 +2354,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="5" t="s">
+      <c r="A146" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B146">
@@ -2364,7 +2368,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="5" t="s">
+      <c r="A147" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B147">
@@ -2378,7 +2382,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="5" t="s">
+      <c r="A148" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B148">
@@ -2392,7 +2396,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="5" t="s">
+      <c r="A149" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B149">
@@ -2406,7 +2410,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="5" t="s">
+      <c r="A150" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B150">
@@ -2420,7 +2424,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="5" t="s">
+      <c r="A151" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B151">
@@ -2434,7 +2438,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="5" t="s">
+      <c r="A152" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B152">
@@ -2448,7 +2452,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="5" t="s">
+      <c r="A153" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B153">
@@ -2462,7 +2466,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="5" t="s">
+      <c r="A154" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B154">
@@ -2476,7 +2480,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="5" t="s">
+      <c r="A155" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B155">
@@ -2490,7 +2494,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="5" t="s">
+      <c r="A156" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B156">
@@ -2504,7 +2508,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="5" t="s">
+      <c r="A157" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B157">
@@ -2518,7 +2522,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="5" t="s">
+      <c r="A158" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B158">
@@ -2532,7 +2536,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="5" t="s">
+      <c r="A159" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B159">
@@ -2546,7 +2550,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="5" t="s">
+      <c r="A160" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B160">
@@ -2560,7 +2564,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="5" t="s">
+      <c r="A161" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B161">
@@ -2574,7 +2578,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="5" t="s">
+      <c r="A162" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B162">
@@ -2588,7 +2592,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="5" t="s">
+      <c r="A163" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B163">
@@ -2602,7 +2606,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="5" t="s">
+      <c r="A164" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B164">
@@ -2616,7 +2620,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="5" t="s">
+      <c r="A165" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B165">
@@ -2630,7 +2634,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="5" t="s">
+      <c r="A166" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B166">
@@ -2644,7 +2648,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="5" t="s">
+      <c r="A167" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B167">
@@ -2658,7 +2662,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="5" t="s">
+      <c r="A168" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B168">
@@ -2672,7 +2676,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="5" t="s">
+      <c r="A169" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B169">
@@ -2686,7 +2690,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="5" t="s">
+      <c r="A170" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B170">
@@ -2700,7 +2704,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="5" t="s">
+      <c r="A171" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B171">
@@ -2714,7 +2718,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="5" t="s">
+      <c r="A172" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B172">
@@ -2728,7 +2732,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="5" t="s">
+      <c r="A173" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B173">
@@ -2742,7 +2746,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="5" t="s">
+      <c r="A174" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B174">
@@ -2756,7 +2760,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="5" t="s">
+      <c r="A175" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B175">
@@ -2770,7 +2774,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="5" t="s">
+      <c r="A176" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B176">
@@ -2784,7 +2788,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="5" t="s">
+      <c r="A177" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B177">
@@ -2798,7 +2802,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="5" t="s">
+      <c r="A178" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B178">
@@ -2812,7 +2816,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="5" t="s">
+      <c r="A179" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B179">
@@ -2826,7 +2830,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="5" t="s">
+      <c r="A180" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B180">
@@ -2840,7 +2844,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="5" t="s">
+      <c r="A181" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B181">
@@ -2854,7 +2858,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="5" t="s">
+      <c r="A182" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B182">
@@ -2868,7 +2872,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="5" t="s">
+      <c r="A183" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B183">
@@ -2882,7 +2886,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="5" t="s">
+      <c r="A184" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B184">
@@ -2896,7 +2900,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="5" t="s">
+      <c r="A185" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B185">
@@ -2910,7 +2914,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="5" t="s">
+      <c r="A186" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B186">
@@ -2924,7 +2928,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="5" t="s">
+      <c r="A187" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B187">
@@ -2938,7 +2942,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="5" t="s">
+      <c r="A188" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B188">
@@ -2952,7 +2956,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="5" t="s">
+      <c r="A189" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B189">
@@ -2966,7 +2970,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="5" t="s">
+      <c r="A190" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B190">
@@ -2980,7 +2984,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="5" t="s">
+      <c r="A191" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B191">
@@ -2994,7 +2998,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="5" t="s">
+      <c r="A192" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B192">
@@ -3008,7 +3012,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="5" t="s">
+      <c r="A193" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B193">
@@ -3022,7 +3026,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="5" t="s">
+      <c r="A194" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B194">
@@ -3036,7 +3040,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="5" t="s">
+      <c r="A195" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B195">
@@ -3050,7 +3054,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="5" t="s">
+      <c r="A196" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B196">
@@ -3064,7 +3068,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="5" t="s">
+      <c r="A197" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B197">
@@ -3078,7 +3082,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="5" t="s">
+      <c r="A198" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B198">
@@ -3092,7 +3096,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="5" t="s">
+      <c r="A199" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B199">
@@ -3106,7 +3110,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="5" t="s">
+      <c r="A200" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B200">
@@ -3120,7 +3124,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="5" t="s">
+      <c r="A201" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B201">
@@ -3134,7 +3138,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="5" t="s">
+      <c r="A202" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B202">
@@ -3148,7 +3152,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="5" t="s">
+      <c r="A203" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B203">
@@ -3162,7 +3166,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="5" t="s">
+      <c r="A204" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B204">
@@ -3176,7 +3180,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="5" t="s">
+      <c r="A205" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B205">
@@ -3190,7 +3194,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="5" t="s">
+      <c r="A206" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B206">
@@ -3204,7 +3208,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="5" t="s">
+      <c r="A207" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B207">
@@ -3218,7 +3222,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="5" t="s">
+      <c r="A208" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B208">
@@ -3232,7 +3236,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="5" t="s">
+      <c r="A209" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B209">
@@ -3246,7 +3250,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="5" t="s">
+      <c r="A210" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B210">
@@ -3260,7 +3264,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="5" t="s">
+      <c r="A211" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B211">
@@ -3274,7 +3278,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="5" t="s">
+      <c r="A212" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B212">
@@ -3288,7 +3292,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="5" t="s">
+      <c r="A213" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B213">
@@ -3302,7 +3306,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="5" t="s">
+      <c r="A214" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B214">
@@ -3316,7 +3320,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="5" t="s">
+      <c r="A215" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B215">
@@ -3330,7 +3334,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="5" t="s">
+      <c r="A216" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B216">
@@ -3344,7 +3348,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="5" t="s">
+      <c r="A217" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B217">
@@ -3358,7 +3362,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="5" t="s">
+      <c r="A218" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B218">
@@ -3372,7 +3376,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="5" t="s">
+      <c r="A219" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B219">
@@ -3386,7 +3390,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="5" t="s">
+      <c r="A220" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B220">
@@ -3400,7 +3404,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="5" t="s">
+      <c r="A221" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B221">
@@ -3414,7 +3418,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="5" t="s">
+      <c r="A222" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B222">
@@ -3428,7 +3432,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="5" t="s">
+      <c r="A223" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B223">
@@ -3442,7 +3446,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="5" t="s">
+      <c r="A224" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B224">
@@ -3456,7 +3460,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="5" t="s">
+      <c r="A225" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B225">
@@ -3470,7 +3474,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="5" t="s">
+      <c r="A226" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B226">
@@ -3484,7 +3488,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="5" t="s">
+      <c r="A227" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B227">
@@ -3498,7 +3502,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="5" t="s">
+      <c r="A228" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B228">
@@ -3512,7 +3516,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="5" t="s">
+      <c r="A229" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B229">
@@ -3526,7 +3530,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="5" t="s">
+      <c r="A230" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B230">
@@ -3540,7 +3544,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="5" t="s">
+      <c r="A231" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B231">
@@ -3554,7 +3558,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="5" t="s">
+      <c r="A232" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B232">
@@ -3568,7 +3572,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B233">
@@ -3582,7 +3586,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="5" t="s">
+      <c r="A234" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B234">
@@ -3596,7 +3600,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="5" t="s">
+      <c r="A235" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B235">
@@ -3610,7 +3614,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="5" t="s">
+      <c r="A236" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B236">
@@ -3624,7 +3628,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="5" t="s">
+      <c r="A237" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B237">
@@ -3638,7 +3642,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="5" t="s">
+      <c r="A238" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B238">
@@ -3652,7 +3656,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="5" t="s">
+      <c r="A239" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B239">
@@ -3666,7 +3670,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="5" t="s">
+      <c r="A240" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B240">
@@ -3680,7 +3684,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="5" t="s">
+      <c r="A241" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B241">
@@ -3694,7 +3698,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="5" t="s">
+      <c r="A242" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B242">
@@ -3708,7 +3712,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="5" t="s">
+      <c r="A243" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B243">
@@ -3722,7 +3726,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="5" t="s">
+      <c r="A244" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B244">
@@ -3736,7 +3740,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="5" t="s">
+      <c r="A245" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B245">
@@ -3750,7 +3754,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="5" t="s">
+      <c r="A246" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B246">
@@ -3764,7 +3768,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="5" t="s">
+      <c r="A247" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B247">
@@ -3778,7 +3782,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="5" t="s">
+      <c r="A248" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B248">
@@ -3792,7 +3796,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="5" t="s">
+      <c r="A249" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B249">
@@ -3806,7 +3810,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="5" t="s">
+      <c r="A250" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B250">
@@ -3820,7 +3824,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="5" t="s">
+      <c r="A251" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B251">
@@ -3834,7 +3838,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="5" t="s">
+      <c r="A252" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B252">
@@ -3848,7 +3852,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="5" t="s">
+      <c r="A253" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B253">
@@ -3862,7 +3866,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="5" t="s">
+      <c r="A254" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B254">
@@ -3876,7 +3880,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="5" t="s">
+      <c r="A255" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B255">
@@ -3890,7 +3894,7 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="5" t="s">
+      <c r="A256" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B256">
@@ -3904,7 +3908,7 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="5" t="s">
+      <c r="A257" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B257">
@@ -3918,7 +3922,7 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="5" t="s">
+      <c r="A258" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B258">
@@ -3932,7 +3936,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="5" t="s">
+      <c r="A259" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B259">
@@ -3946,7 +3950,7 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="5" t="s">
+      <c r="A260" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B260">
@@ -3960,7 +3964,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="5" t="s">
+      <c r="A261" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B261">
@@ -3974,7 +3978,7 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="5" t="s">
+      <c r="A262" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B262">
@@ -3988,7 +3992,7 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="5" t="s">
+      <c r="A263" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B263">
@@ -4002,7 +4006,7 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="5" t="s">
+      <c r="A264" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B264">
@@ -4016,7 +4020,7 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="5" t="s">
+      <c r="A265" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B265">
@@ -4030,7 +4034,7 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="5" t="s">
+      <c r="A266" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B266">
@@ -4044,7 +4048,7 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="5" t="s">
+      <c r="A267" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B267">
@@ -4058,7 +4062,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="5" t="s">
+      <c r="A268" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B268">
@@ -4072,7 +4076,7 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="5" t="s">
+      <c r="A269" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B269">
@@ -4086,7 +4090,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="5" t="s">
+      <c r="A270" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B270">
@@ -4100,7 +4104,7 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="5" t="s">
+      <c r="A271" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B271">
@@ -4114,7 +4118,7 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="5" t="s">
+      <c r="A272" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B272">
@@ -4128,7 +4132,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="5" t="s">
+      <c r="A273" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B273">
@@ -4142,7 +4146,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="5" t="s">
+      <c r="A274" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B274">
@@ -4156,7 +4160,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="5" t="s">
+      <c r="A275" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B275">
@@ -4170,7 +4174,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="5" t="s">
+      <c r="A276" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B276">
@@ -4184,7 +4188,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="5" t="s">
+      <c r="A277" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B277">
@@ -4198,7 +4202,7 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="5" t="s">
+      <c r="A278" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B278">
@@ -4212,7 +4216,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="5" t="s">
+      <c r="A279" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B279">
@@ -4226,7 +4230,7 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="5" t="s">
+      <c r="A280" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B280">
@@ -4240,7 +4244,7 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="5" t="s">
+      <c r="A281" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B281">
@@ -4254,7 +4258,7 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="5" t="s">
+      <c r="A282" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B282">
@@ -4268,7 +4272,7 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="5" t="s">
+      <c r="A283" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B283">
@@ -4282,7 +4286,7 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="5" t="s">
+      <c r="A284" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B284">
@@ -4296,7 +4300,7 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="5" t="s">
+      <c r="A285" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B285">
@@ -4310,7 +4314,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="5" t="s">
+      <c r="A286" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B286">
@@ -4324,7 +4328,7 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="5" t="s">
+      <c r="A287" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B287">
@@ -4338,7 +4342,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="5" t="s">
+      <c r="A288" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B288">
@@ -4352,7 +4356,7 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="5" t="s">
+      <c r="A289" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B289">
@@ -4366,7 +4370,7 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="5" t="s">
+      <c r="A290" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B290">
@@ -4380,7 +4384,7 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="5" t="s">
+      <c r="A291" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B291">
@@ -4394,7 +4398,7 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="5" t="s">
+      <c r="A292" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B292">
@@ -4408,7 +4412,7 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="5" t="s">
+      <c r="A293" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B293">
@@ -4422,7 +4426,7 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="5" t="s">
+      <c r="A294" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B294">
@@ -4436,7 +4440,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="5" t="s">
+      <c r="A295" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B295">
@@ -4450,7 +4454,7 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="5" t="s">
+      <c r="A296" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B296">
@@ -4464,7 +4468,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="5" t="s">
+      <c r="A297" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B297">
@@ -4478,7 +4482,7 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="5" t="s">
+      <c r="A298" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B298">
@@ -4492,7 +4496,7 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" s="5" t="s">
+      <c r="A299" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B299">
@@ -4506,7 +4510,7 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" s="5" t="s">
+      <c r="A300" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B300">
@@ -4520,7 +4524,7 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" s="5" t="s">
+      <c r="A301" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B301">
@@ -4534,7 +4538,7 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" s="5" t="s">
+      <c r="A302" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B302">
@@ -4548,7 +4552,7 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" s="5" t="s">
+      <c r="A303" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B303">
@@ -4562,7 +4566,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="5" t="s">
+      <c r="A304" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B304">
@@ -4576,7 +4580,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="5" t="s">
+      <c r="A305" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B305">
@@ -4590,7 +4594,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="5" t="s">
+      <c r="A306" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B306">
@@ -4604,7 +4608,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="5" t="s">
+      <c r="A307" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B307">
@@ -4618,7 +4622,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="5" t="s">
+      <c r="A308" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B308">
@@ -4632,7 +4636,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="5" t="s">
+      <c r="A309" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B309">
@@ -4646,7 +4650,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="5" t="s">
+      <c r="A310" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B310">
@@ -4660,7 +4664,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="5" t="s">
+      <c r="A311" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B311">
@@ -4674,7 +4678,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="5" t="s">
+      <c r="A312" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B312">
@@ -4688,7 +4692,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="5" t="s">
+      <c r="A313" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B313">
@@ -4702,7 +4706,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="5" t="s">
+      <c r="A314" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B314">
@@ -4716,7 +4720,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="5" t="s">
+      <c r="A315" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B315">
@@ -4730,7 +4734,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="5" t="s">
+      <c r="A316" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B316">
@@ -4744,7 +4748,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="5" t="s">
+      <c r="A317" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B317">
@@ -4758,7 +4762,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="5" t="s">
+      <c r="A318" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B318">
@@ -4772,7 +4776,7 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" s="5" t="s">
+      <c r="A319" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B319">
@@ -4786,7 +4790,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="5" t="s">
+      <c r="A320" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B320">
@@ -4800,7 +4804,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="5" t="s">
+      <c r="A321" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B321">
@@ -4814,7 +4818,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="5" t="s">
+      <c r="A322" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B322">
@@ -4828,7 +4832,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="5" t="s">
+      <c r="A323" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B323">
@@ -4842,7 +4846,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="5" t="s">
+      <c r="A324" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B324">
@@ -4856,7 +4860,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="5" t="s">
+      <c r="A325" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B325">
@@ -4870,7 +4874,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="5" t="s">
+      <c r="A326" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B326">
@@ -4884,7 +4888,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="5" t="s">
+      <c r="A327" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B327">
@@ -4898,7 +4902,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="5" t="s">
+      <c r="A328" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B328">
@@ -4912,7 +4916,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="5" t="s">
+      <c r="A329" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B329">
@@ -4926,7 +4930,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="5" t="s">
+      <c r="A330" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B330">
@@ -4940,7 +4944,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="5" t="s">
+      <c r="A331" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B331">
@@ -4954,7 +4958,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="5" t="s">
+      <c r="A332" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B332">
@@ -4968,7 +4972,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="5" t="s">
+      <c r="A333" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B333">
@@ -4982,7 +4986,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="5" t="s">
+      <c r="A334" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B334">
@@ -4996,7 +5000,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="5" t="s">
+      <c r="A335" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B335">
@@ -5010,7 +5014,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="5" t="s">
+      <c r="A336" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B336">
@@ -5024,7 +5028,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="5" t="s">
+      <c r="A337" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B337">
@@ -5038,7 +5042,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="5" t="s">
+      <c r="A338" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B338">
@@ -5052,7 +5056,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="5" t="s">
+      <c r="A339" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B339">
@@ -5066,7 +5070,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="5" t="s">
+      <c r="A340" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B340">
@@ -5080,7 +5084,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="5" t="s">
+      <c r="A341" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B341">
@@ -5094,7 +5098,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="5" t="s">
+      <c r="A342" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B342">
@@ -5108,7 +5112,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="5" t="s">
+      <c r="A343" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B343">
@@ -5122,7 +5126,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="5" t="s">
+      <c r="A344" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B344">
@@ -5136,7 +5140,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="5" t="s">
+      <c r="A345" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B345">
@@ -5150,7 +5154,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="5" t="s">
+      <c r="A346" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B346">
@@ -5164,7 +5168,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="5" t="s">
+      <c r="A347" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B347">
@@ -5178,7 +5182,7 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" s="5" t="s">
+      <c r="A348" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B348">
@@ -5192,7 +5196,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="5" t="s">
+      <c r="A349" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B349">
@@ -5206,7 +5210,7 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" s="5" t="s">
+      <c r="A350" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B350">
@@ -5220,7 +5224,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" s="5" t="s">
+      <c r="A351" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B351">
@@ -5234,7 +5238,7 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="5" t="s">
+      <c r="A352" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B352">
@@ -5248,7 +5252,7 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="5" t="s">
+      <c r="A353" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B353">
@@ -5262,7 +5266,7 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" s="5" t="s">
+      <c r="A354" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B354">
@@ -5276,7 +5280,7 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" s="5" t="s">
+      <c r="A355" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B355">
@@ -5290,7 +5294,7 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" s="5" t="s">
+      <c r="A356" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B356">
@@ -5304,7 +5308,7 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" s="5" t="s">
+      <c r="A357" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B357">
@@ -5318,7 +5322,7 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" s="5" t="s">
+      <c r="A358" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B358">
@@ -5332,7 +5336,7 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" s="5" t="s">
+      <c r="A359" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B359">
@@ -5346,7 +5350,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" s="5" t="s">
+      <c r="A360" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B360">
@@ -5360,7 +5364,7 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" s="5" t="s">
+      <c r="A361" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B361">
@@ -5374,7 +5378,7 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" s="5" t="s">
+      <c r="A362" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B362">
@@ -5388,7 +5392,7 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" s="5" t="s">
+      <c r="A363" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B363">
@@ -5402,7 +5406,7 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" s="5" t="s">
+      <c r="A364" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B364">
@@ -5416,7 +5420,7 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" s="5" t="s">
+      <c r="A365" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B365">
@@ -5430,7 +5434,7 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" s="5" t="s">
+      <c r="A366" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B366">
@@ -5444,7 +5448,7 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" s="5" t="s">
+      <c r="A367" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B367">
@@ -5458,7 +5462,7 @@
       </c>
     </row>
     <row r="368">
-      <c r="A368" s="5" t="s">
+      <c r="A368" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B368">
@@ -5472,7 +5476,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" s="5" t="s">
+      <c r="A369" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B369">
@@ -5486,7 +5490,7 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" s="5" t="s">
+      <c r="A370" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B370">
@@ -5500,7 +5504,7 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" s="5" t="s">
+      <c r="A371" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B371">
@@ -5514,7 +5518,7 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" s="5" t="s">
+      <c r="A372" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B372">
@@ -5528,7 +5532,7 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" s="5" t="s">
+      <c r="A373" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B373">
@@ -5542,7 +5546,7 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" s="5" t="s">
+      <c r="A374" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B374">
@@ -5556,7 +5560,7 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" s="5" t="s">
+      <c r="A375" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B375">
@@ -5570,7 +5574,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="5" t="s">
+      <c r="A376" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B376">
@@ -5584,7 +5588,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="5" t="s">
+      <c r="A377" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B377">
@@ -5598,7 +5602,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="5" t="s">
+      <c r="A378" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B378">
@@ -5612,7 +5616,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="5" t="s">
+      <c r="A379" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B379">
@@ -5626,7 +5630,7 @@
       </c>
     </row>
     <row r="380">
-      <c r="A380" s="5" t="s">
+      <c r="A380" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B380">
@@ -5640,7 +5644,7 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" s="5" t="s">
+      <c r="A381" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B381">
@@ -5654,7 +5658,7 @@
       </c>
     </row>
     <row r="382">
-      <c r="A382" s="5" t="s">
+      <c r="A382" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B382">
@@ -5668,7 +5672,7 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" s="5" t="s">
+      <c r="A383" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B383">
@@ -5682,7 +5686,7 @@
       </c>
     </row>
     <row r="384">
-      <c r="A384" s="5" t="s">
+      <c r="A384" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B384">
@@ -5696,7 +5700,7 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" s="5" t="s">
+      <c r="A385" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B385">
@@ -5710,7 +5714,7 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" s="5" t="s">
+      <c r="A386" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B386">
@@ -5724,7 +5728,7 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" s="5" t="s">
+      <c r="A387" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B387">
@@ -5738,7 +5742,7 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" s="5" t="s">
+      <c r="A388" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B388">
@@ -5752,7 +5756,7 @@
       </c>
     </row>
     <row r="389">
-      <c r="A389" s="5" t="s">
+      <c r="A389" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B389">
@@ -5766,7 +5770,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" s="5" t="s">
+      <c r="A390" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B390">
@@ -5780,7 +5784,7 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" s="5" t="s">
+      <c r="A391" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B391">
@@ -5794,7 +5798,7 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" s="5" t="s">
+      <c r="A392" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B392">
@@ -5808,7 +5812,7 @@
       </c>
     </row>
     <row r="393">
-      <c r="A393" s="5" t="s">
+      <c r="A393" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B393">
@@ -5822,7 +5826,7 @@
       </c>
     </row>
     <row r="394">
-      <c r="A394" s="5" t="s">
+      <c r="A394" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B394">
@@ -5836,7 +5840,7 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" s="5" t="s">
+      <c r="A395" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B395">
@@ -5850,7 +5854,7 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="5" t="s">
+      <c r="A396" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B396">
@@ -5864,7 +5868,7 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="5" t="s">
+      <c r="A397" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B397">
@@ -5878,7 +5882,7 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" s="5" t="s">
+      <c r="A398" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B398">
@@ -5892,7 +5896,7 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" s="5" t="s">
+      <c r="A399" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B399">
@@ -5906,7 +5910,7 @@
       </c>
     </row>
     <row r="400">
-      <c r="A400" s="5" t="s">
+      <c r="A400" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B400">
@@ -5920,7 +5924,7 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" s="5" t="s">
+      <c r="A401" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B401">
@@ -5934,7 +5938,7 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="5" t="s">
+      <c r="A402" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B402">
@@ -5948,7 +5952,7 @@
       </c>
     </row>
     <row r="403">
-      <c r="A403" s="5" t="s">
+      <c r="A403" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B403">
@@ -5962,7 +5966,7 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="5" t="s">
+      <c r="A404" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B404">
@@ -5976,7 +5980,7 @@
       </c>
     </row>
     <row r="405">
-      <c r="A405" s="5" t="s">
+      <c r="A405" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B405">
@@ -5990,7 +5994,7 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="5" t="s">
+      <c r="A406" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B406">
@@ -6004,7 +6008,7 @@
       </c>
     </row>
     <row r="407">
-      <c r="A407" s="5" t="s">
+      <c r="A407" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B407">
@@ -6018,7 +6022,7 @@
       </c>
     </row>
     <row r="408">
-      <c r="A408" s="5" t="s">
+      <c r="A408" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B408">
@@ -6032,7 +6036,7 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="5" t="s">
+      <c r="A409" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B409">
@@ -6046,7 +6050,7 @@
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="5" t="s">
+      <c r="A410" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B410">
@@ -6060,7 +6064,7 @@
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="5" t="s">
+      <c r="A411" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B411">
@@ -6074,7 +6078,7 @@
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="5" t="s">
+      <c r="A412" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B412">
@@ -6088,7 +6092,7 @@
       </c>
     </row>
     <row r="413">
-      <c r="A413" s="5" t="s">
+      <c r="A413" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B413">
@@ -6102,7 +6106,7 @@
       </c>
     </row>
     <row r="414">
-      <c r="A414" s="5" t="s">
+      <c r="A414" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B414">
@@ -6116,7 +6120,7 @@
       </c>
     </row>
     <row r="415">
-      <c r="A415" s="5" t="s">
+      <c r="A415" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B415">
@@ -6130,7 +6134,7 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="5" t="s">
+      <c r="A416" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B416">
@@ -6144,7 +6148,7 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="5" t="s">
+      <c r="A417" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B417">
@@ -6158,7 +6162,7 @@
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="5" t="s">
+      <c r="A418" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B418">
@@ -6172,7 +6176,7 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" s="5" t="s">
+      <c r="A419" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B419">
@@ -6186,7 +6190,7 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" s="5" t="s">
+      <c r="A420" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B420">
@@ -6200,7 +6204,7 @@
       </c>
     </row>
     <row r="421">
-      <c r="A421" s="5" t="s">
+      <c r="A421" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B421">
@@ -6214,7 +6218,7 @@
       </c>
     </row>
     <row r="422">
-      <c r="A422" s="5" t="s">
+      <c r="A422" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B422">
@@ -6228,7 +6232,7 @@
       </c>
     </row>
     <row r="423">
-      <c r="A423" s="5" t="s">
+      <c r="A423" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B423">
@@ -6242,7 +6246,7 @@
       </c>
     </row>
     <row r="424">
-      <c r="A424" s="5" t="s">
+      <c r="A424" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B424">
@@ -6256,7 +6260,7 @@
       </c>
     </row>
     <row r="425">
-      <c r="A425" s="5" t="s">
+      <c r="A425" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B425">
@@ -6270,7 +6274,7 @@
       </c>
     </row>
     <row r="426">
-      <c r="A426" s="5" t="s">
+      <c r="A426" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B426">
@@ -6284,7 +6288,7 @@
       </c>
     </row>
     <row r="427">
-      <c r="A427" s="5" t="s">
+      <c r="A427" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B427">
@@ -6298,7 +6302,7 @@
       </c>
     </row>
     <row r="428">
-      <c r="A428" s="5" t="s">
+      <c r="A428" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B428">
@@ -6312,7 +6316,7 @@
       </c>
     </row>
     <row r="429">
-      <c r="A429" s="5" t="s">
+      <c r="A429" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B429">
@@ -6326,7 +6330,7 @@
       </c>
     </row>
     <row r="430">
-      <c r="A430" s="5" t="s">
+      <c r="A430" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B430">
@@ -6340,7 +6344,7 @@
       </c>
     </row>
     <row r="431">
-      <c r="A431" s="5" t="s">
+      <c r="A431" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B431">
@@ -6354,7 +6358,7 @@
       </c>
     </row>
     <row r="432">
-      <c r="A432" s="5" t="s">
+      <c r="A432" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B432">
@@ -6368,7 +6372,7 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" s="5" t="s">
+      <c r="A433" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B433">
@@ -6382,7 +6386,7 @@
       </c>
     </row>
     <row r="434">
-      <c r="A434" s="5" t="s">
+      <c r="A434" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B434">
@@ -6396,7 +6400,7 @@
       </c>
     </row>
     <row r="435">
-      <c r="A435" s="5" t="s">
+      <c r="A435" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B435">
@@ -6410,7 +6414,7 @@
       </c>
     </row>
     <row r="436">
-      <c r="A436" s="5" t="s">
+      <c r="A436" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B436">
@@ -6424,7 +6428,7 @@
       </c>
     </row>
     <row r="437">
-      <c r="A437" s="5" t="s">
+      <c r="A437" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B437">
@@ -6438,7 +6442,7 @@
       </c>
     </row>
     <row r="438">
-      <c r="A438" s="5" t="s">
+      <c r="A438" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B438">
@@ -6452,7 +6456,7 @@
       </c>
     </row>
     <row r="439">
-      <c r="A439" s="5" t="s">
+      <c r="A439" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B439">
@@ -6466,7 +6470,7 @@
       </c>
     </row>
     <row r="440">
-      <c r="A440" s="5" t="s">
+      <c r="A440" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B440">
@@ -6480,7 +6484,7 @@
       </c>
     </row>
     <row r="441">
-      <c r="A441" s="5" t="s">
+      <c r="A441" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B441">
@@ -6494,7 +6498,7 @@
       </c>
     </row>
     <row r="442">
-      <c r="A442" s="5" t="s">
+      <c r="A442" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B442">
@@ -6508,7 +6512,7 @@
       </c>
     </row>
     <row r="443">
-      <c r="A443" s="5" t="s">
+      <c r="A443" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B443">
@@ -6522,7 +6526,7 @@
       </c>
     </row>
     <row r="444">
-      <c r="A444" s="5" t="s">
+      <c r="A444" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B444">
@@ -6536,7 +6540,7 @@
       </c>
     </row>
     <row r="445">
-      <c r="A445" s="5" t="s">
+      <c r="A445" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B445">
@@ -6550,7 +6554,7 @@
       </c>
     </row>
     <row r="446">
-      <c r="A446" s="5" t="s">
+      <c r="A446" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B446">
@@ -6564,7 +6568,7 @@
       </c>
     </row>
     <row r="447">
-      <c r="A447" s="5" t="s">
+      <c r="A447" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B447">
@@ -6578,7 +6582,7 @@
       </c>
     </row>
     <row r="448">
-      <c r="A448" s="5" t="s">
+      <c r="A448" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B448">
@@ -6592,7 +6596,7 @@
       </c>
     </row>
     <row r="449">
-      <c r="A449" s="5" t="s">
+      <c r="A449" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B449">
@@ -6606,7 +6610,7 @@
       </c>
     </row>
     <row r="450">
-      <c r="A450" s="5" t="s">
+      <c r="A450" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B450">
@@ -6620,7 +6624,7 @@
       </c>
     </row>
     <row r="451">
-      <c r="A451" s="5" t="s">
+      <c r="A451" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B451">
@@ -6634,7 +6638,7 @@
       </c>
     </row>
     <row r="452">
-      <c r="A452" s="5" t="s">
+      <c r="A452" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B452">
@@ -6648,7 +6652,7 @@
       </c>
     </row>
     <row r="453">
-      <c r="A453" s="5" t="s">
+      <c r="A453" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B453">
@@ -6662,7 +6666,7 @@
       </c>
     </row>
     <row r="454">
-      <c r="A454" s="5" t="s">
+      <c r="A454" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B454">
@@ -6676,7 +6680,7 @@
       </c>
     </row>
     <row r="455">
-      <c r="A455" s="5" t="s">
+      <c r="A455" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B455">
@@ -6690,7 +6694,7 @@
       </c>
     </row>
     <row r="456">
-      <c r="A456" s="5" t="s">
+      <c r="A456" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B456">
@@ -6704,7 +6708,7 @@
       </c>
     </row>
     <row r="457">
-      <c r="A457" s="5" t="s">
+      <c r="A457" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B457">
@@ -6718,7 +6722,7 @@
       </c>
     </row>
     <row r="458">
-      <c r="A458" s="5" t="s">
+      <c r="A458" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B458">
@@ -6732,7 +6736,7 @@
       </c>
     </row>
     <row r="459">
-      <c r="A459" s="5" t="s">
+      <c r="A459" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B459">
@@ -6746,7 +6750,7 @@
       </c>
     </row>
     <row r="460">
-      <c r="A460" s="5" t="s">
+      <c r="A460" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B460">
@@ -6760,7 +6764,7 @@
       </c>
     </row>
     <row r="461">
-      <c r="A461" s="5" t="s">
+      <c r="A461" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B461">
@@ -6774,7 +6778,7 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" s="5" t="s">
+      <c r="A462" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B462">
@@ -6788,7 +6792,7 @@
       </c>
     </row>
     <row r="463">
-      <c r="A463" s="5" t="s">
+      <c r="A463" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B463">
@@ -6802,7 +6806,7 @@
       </c>
     </row>
     <row r="464">
-      <c r="A464" s="5" t="s">
+      <c r="A464" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B464">
@@ -6816,7 +6820,7 @@
       </c>
     </row>
     <row r="465">
-      <c r="A465" s="5" t="s">
+      <c r="A465" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B465">
@@ -6830,7 +6834,7 @@
       </c>
     </row>
     <row r="466">
-      <c r="A466" s="5" t="s">
+      <c r="A466" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B466">
@@ -6844,7 +6848,7 @@
       </c>
     </row>
     <row r="467">
-      <c r="A467" s="5" t="s">
+      <c r="A467" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B467">
@@ -6858,7 +6862,7 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" s="5" t="s">
+      <c r="A468" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B468">
@@ -6872,7 +6876,7 @@
       </c>
     </row>
     <row r="469">
-      <c r="A469" s="5" t="s">
+      <c r="A469" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B469">
@@ -6886,7 +6890,7 @@
       </c>
     </row>
     <row r="470">
-      <c r="A470" s="5" t="s">
+      <c r="A470" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B470">
@@ -6900,7 +6904,7 @@
       </c>
     </row>
     <row r="471">
-      <c r="A471" s="5" t="s">
+      <c r="A471" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B471">
@@ -6914,7 +6918,7 @@
       </c>
     </row>
     <row r="472">
-      <c r="A472" s="5" t="s">
+      <c r="A472" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B472">
@@ -6928,7 +6932,7 @@
       </c>
     </row>
     <row r="473">
-      <c r="A473" s="5" t="s">
+      <c r="A473" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B473">
@@ -6942,7 +6946,7 @@
       </c>
     </row>
     <row r="474">
-      <c r="A474" s="5" t="s">
+      <c r="A474" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B474">
@@ -6956,7 +6960,7 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" s="5" t="s">
+      <c r="A475" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B475">
@@ -6970,7 +6974,7 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" s="5" t="s">
+      <c r="A476" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B476">
@@ -6984,7 +6988,7 @@
       </c>
     </row>
     <row r="477">
-      <c r="A477" s="5" t="s">
+      <c r="A477" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B477">
@@ -6998,7 +7002,7 @@
       </c>
     </row>
     <row r="478">
-      <c r="A478" s="5" t="s">
+      <c r="A478" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B478">
@@ -7012,7 +7016,7 @@
       </c>
     </row>
     <row r="479">
-      <c r="A479" s="5" t="s">
+      <c r="A479" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B479">
@@ -7026,7 +7030,7 @@
       </c>
     </row>
     <row r="480">
-      <c r="A480" s="5" t="s">
+      <c r="A480" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B480">
@@ -7040,7 +7044,7 @@
       </c>
     </row>
     <row r="481">
-      <c r="A481" s="5" t="s">
+      <c r="A481" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B481">
@@ -7054,7 +7058,7 @@
       </c>
     </row>
     <row r="482">
-      <c r="A482" s="5" t="s">
+      <c r="A482" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B482">
@@ -7068,7 +7072,7 @@
       </c>
     </row>
     <row r="483">
-      <c r="A483" s="5" t="s">
+      <c r="A483" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B483">
@@ -7082,7 +7086,7 @@
       </c>
     </row>
     <row r="484">
-      <c r="A484" s="5" t="s">
+      <c r="A484" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B484">
@@ -7096,7 +7100,7 @@
       </c>
     </row>
     <row r="485">
-      <c r="A485" s="5" t="s">
+      <c r="A485" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B485">
@@ -7110,7 +7114,7 @@
       </c>
     </row>
     <row r="486">
-      <c r="A486" s="5" t="s">
+      <c r="A486" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B486">
@@ -7124,7 +7128,7 @@
       </c>
     </row>
     <row r="487">
-      <c r="A487" s="5" t="s">
+      <c r="A487" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B487">
@@ -7138,7 +7142,7 @@
       </c>
     </row>
     <row r="488">
-      <c r="A488" s="5" t="s">
+      <c r="A488" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B488">
@@ -7152,7 +7156,7 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" s="5" t="s">
+      <c r="A489" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B489">
@@ -7166,7 +7170,7 @@
       </c>
     </row>
     <row r="490">
-      <c r="A490" s="5" t="s">
+      <c r="A490" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B490">
@@ -7180,7 +7184,7 @@
       </c>
     </row>
     <row r="491">
-      <c r="A491" s="5" t="s">
+      <c r="A491" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B491">
@@ -7194,7 +7198,7 @@
       </c>
     </row>
     <row r="492">
-      <c r="A492" s="5" t="s">
+      <c r="A492" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B492">
@@ -7208,7 +7212,7 @@
       </c>
     </row>
     <row r="493">
-      <c r="A493" s="5" t="s">
+      <c r="A493" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B493">
@@ -7222,7 +7226,7 @@
       </c>
     </row>
     <row r="494">
-      <c r="A494" s="5" t="s">
+      <c r="A494" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B494">
@@ -7236,7 +7240,7 @@
       </c>
     </row>
     <row r="495">
-      <c r="A495" s="5" t="s">
+      <c r="A495" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B495">
@@ -7250,7 +7254,7 @@
       </c>
     </row>
     <row r="496">
-      <c r="A496" s="5" t="s">
+      <c r="A496" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B496">
@@ -7264,7 +7268,7 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="5" t="s">
+      <c r="A497" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B497">
@@ -7278,7 +7282,7 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="5" t="s">
+      <c r="A498" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B498">
@@ -7292,7 +7296,7 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="5" t="s">
+      <c r="A499" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B499">
@@ -7306,7 +7310,7 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="5" t="s">
+      <c r="A500" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B500">
@@ -7320,7 +7324,7 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="5" t="s">
+      <c r="A501" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B501">
@@ -7334,7 +7338,7 @@
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="5" t="s">
+      <c r="A502" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B502">
@@ -7348,7 +7352,7 @@
       </c>
     </row>
     <row r="503">
-      <c r="A503" s="5" t="s">
+      <c r="A503" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B503">
@@ -7362,7 +7366,7 @@
       </c>
     </row>
     <row r="504">
-      <c r="A504" s="5" t="s">
+      <c r="A504" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B504">
@@ -7376,7 +7380,7 @@
       </c>
     </row>
     <row r="505">
-      <c r="A505" s="5" t="s">
+      <c r="A505" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B505">
@@ -7390,7 +7394,7 @@
       </c>
     </row>
     <row r="506">
-      <c r="A506" s="5" t="s">
+      <c r="A506" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B506">
@@ -7404,7 +7408,7 @@
       </c>
     </row>
     <row r="507">
-      <c r="A507" s="5" t="s">
+      <c r="A507" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B507">
@@ -7418,7 +7422,7 @@
       </c>
     </row>
     <row r="508">
-      <c r="A508" s="5" t="s">
+      <c r="A508" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B508">
@@ -7432,7 +7436,7 @@
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="5" t="s">
+      <c r="A509" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B509">
@@ -7446,7 +7450,7 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="5" t="s">
+      <c r="A510" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B510">
@@ -7460,7 +7464,7 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="5" t="s">
+      <c r="A511" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B511">
@@ -7474,7 +7478,7 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="5" t="s">
+      <c r="A512" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B512">
@@ -7488,7 +7492,7 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="5" t="s">
+      <c r="A513" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B513">
@@ -7502,7 +7506,7 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="5" t="s">
+      <c r="A514" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B514">
@@ -7516,7 +7520,7 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="5" t="s">
+      <c r="A515" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B515">
@@ -7530,7 +7534,7 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="5" t="s">
+      <c r="A516" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B516">
@@ -7544,7 +7548,7 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="5" t="s">
+      <c r="A517" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B517">
@@ -7558,7 +7562,7 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="5" t="s">
+      <c r="A518" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B518">
@@ -7572,7 +7576,7 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="5" t="s">
+      <c r="A519" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B519">
@@ -7586,7 +7590,7 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="5" t="s">
+      <c r="A520" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B520">

</xml_diff>